<commit_message>
change target file form
</commit_message>
<xml_diff>
--- a/excel_files/资金日报汇总表.xlsx
+++ b/excel_files/资金日报汇总表.xlsx
@@ -568,7 +568,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -748,6 +748,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="85">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
@@ -1000,7 +1024,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1140,10 +1164,16 @@
     <xf fontId="25" fillId="0" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="25" fillId="0" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="10" numFmtId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf fontId="21" fillId="0" borderId="10" numFmtId="4" xfId="58" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="10" numFmtId="170" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="25" fillId="0" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="21" fillId="0" borderId="10" numFmtId="170" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3094,75 +3124,73 @@
     </row>
     <row r="10" ht="15">
       <c r="A10" s="14"/>
-      <c r="B10" s="17" t="s">
-        <v>40</v>
-      </c>
+      <c r="B10" s="49"/>
       <c r="C10" s="14">
         <v>1</v>
       </c>
       <c r="D10" s="35"/>
       <c r="E10" s="35"/>
-      <c r="F10" s="49"/>
+      <c r="F10" s="50"/>
       <c r="G10" s="34"/>
     </row>
     <row r="11" ht="15">
       <c r="A11" s="14"/>
-      <c r="B11" s="17"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="14">
         <v>2</v>
       </c>
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>
-      <c r="F11" s="49"/>
+      <c r="F11" s="50"/>
       <c r="G11" s="15"/>
     </row>
     <row r="12" ht="15">
       <c r="A12" s="14"/>
-      <c r="B12" s="17"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="14">
         <v>3</v>
       </c>
       <c r="D12" s="35"/>
       <c r="E12" s="35"/>
-      <c r="F12" s="49"/>
+      <c r="F12" s="50"/>
       <c r="G12" s="15"/>
     </row>
     <row r="13" ht="15">
       <c r="A13" s="14"/>
-      <c r="B13" s="17"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="14">
         <v>4</v>
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="35"/>
-      <c r="F13" s="49"/>
+      <c r="F13" s="50"/>
       <c r="G13" s="15"/>
     </row>
     <row r="14" ht="15">
       <c r="A14" s="14"/>
-      <c r="B14" s="17"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="14">
         <v>5</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="36"/>
-      <c r="F14" s="50"/>
+      <c r="F14" s="51"/>
       <c r="G14" s="15"/>
     </row>
     <row r="15" ht="15">
       <c r="A15" s="14"/>
-      <c r="B15" s="17"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="14">
         <v>6</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="38"/>
-      <c r="F15" s="51"/>
+      <c r="F15" s="52"/>
       <c r="G15" s="15"/>
     </row>
     <row r="16" ht="15">
       <c r="A16" s="14"/>
-      <c r="B16" s="17"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="14">
         <v>7</v>
       </c>
@@ -3173,7 +3201,7 @@
     </row>
     <row r="17" ht="15">
       <c r="A17" s="14"/>
-      <c r="B17" s="17"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="14">
         <v>8</v>
       </c>
@@ -3184,7 +3212,7 @@
     </row>
     <row r="18" ht="15">
       <c r="A18" s="14"/>
-      <c r="B18" s="17"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="14">
         <v>9</v>
       </c>
@@ -3195,7 +3223,7 @@
     </row>
     <row r="19" ht="15">
       <c r="A19" s="14"/>
-      <c r="B19" s="17"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="14">
         <v>10</v>
       </c>
@@ -3206,13 +3234,13 @@
     </row>
     <row r="20" ht="15">
       <c r="A20" s="14"/>
-      <c r="B20" s="17"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="42"/>
       <c r="E20" s="42"/>
-      <c r="F20" s="52"/>
+      <c r="F20" s="54"/>
       <c r="G20" s="15"/>
     </row>
     <row r="21" ht="15">
@@ -3223,7 +3251,7 @@
       <c r="C21" s="44"/>
       <c r="D21" s="44"/>
       <c r="E21" s="44"/>
-      <c r="F21" s="53"/>
+      <c r="F21" s="55"/>
       <c r="G21" s="15"/>
     </row>
     <row r="22" ht="15">
@@ -3249,7 +3277,7 @@
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
-      <c r="F23" s="54"/>
+      <c r="F23" s="56"/>
       <c r="G23" s="15"/>
     </row>
     <row r="24" ht="15">
@@ -3260,7 +3288,7 @@
       </c>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
-      <c r="F24" s="54"/>
+      <c r="F24" s="56"/>
       <c r="G24" s="15"/>
     </row>
     <row r="25" ht="15">
@@ -3271,7 +3299,7 @@
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
-      <c r="F25" s="54"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="15"/>
     </row>
     <row r="26" ht="15">
@@ -3293,7 +3321,7 @@
       </c>
       <c r="D27" s="35"/>
       <c r="E27" s="35"/>
-      <c r="F27" s="54"/>
+      <c r="F27" s="56"/>
       <c r="G27" s="15"/>
     </row>
     <row r="28" ht="15">
@@ -3304,7 +3332,7 @@
       </c>
       <c r="D28" s="35"/>
       <c r="E28" s="35"/>
-      <c r="F28" s="54"/>
+      <c r="F28" s="56"/>
       <c r="G28" s="15"/>
     </row>
     <row r="29" ht="15">
@@ -3315,7 +3343,7 @@
       </c>
       <c r="D29" s="35"/>
       <c r="E29" s="35"/>
-      <c r="F29" s="54"/>
+      <c r="F29" s="56"/>
       <c r="G29" s="15"/>
     </row>
     <row r="30" ht="15">
@@ -3326,7 +3354,7 @@
       </c>
       <c r="D30" s="35"/>
       <c r="E30" s="35"/>
-      <c r="F30" s="54"/>
+      <c r="F30" s="56"/>
       <c r="G30" s="15"/>
     </row>
     <row r="31" ht="15">
@@ -3337,7 +3365,7 @@
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="26"/>
-      <c r="F31" s="54"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="15"/>
     </row>
     <row r="32" ht="15">
@@ -3361,7 +3389,7 @@
       </c>
       <c r="D33" s="35"/>
       <c r="E33" s="35"/>
-      <c r="F33" s="49"/>
+      <c r="F33" s="50"/>
       <c r="G33" s="34"/>
     </row>
     <row r="34" ht="15">
@@ -3372,7 +3400,7 @@
       </c>
       <c r="D34" s="35"/>
       <c r="E34" s="35"/>
-      <c r="F34" s="49"/>
+      <c r="F34" s="50"/>
       <c r="G34" s="15"/>
     </row>
     <row r="35" ht="15">
@@ -3449,7 +3477,7 @@
       </c>
       <c r="D41" s="35"/>
       <c r="E41" s="35"/>
-      <c r="F41" s="49"/>
+      <c r="F41" s="50"/>
       <c r="G41" s="15"/>
     </row>
     <row r="42" ht="15">
@@ -3471,7 +3499,7 @@
       </c>
       <c r="D43" s="26"/>
       <c r="E43" s="26"/>
-      <c r="F43" s="54"/>
+      <c r="F43" s="56"/>
       <c r="G43" s="15"/>
     </row>
     <row r="44" ht="15">
@@ -3482,7 +3510,7 @@
       <c r="C44" s="44"/>
       <c r="D44" s="44"/>
       <c r="E44" s="44"/>
-      <c r="F44" s="53"/>
+      <c r="F44" s="55"/>
       <c r="G44" s="15"/>
     </row>
   </sheetData>
@@ -3491,7 +3519,7 @@
     <mergeCell ref="A2:B8"/>
     <mergeCell ref="E2:E8"/>
     <mergeCell ref="A9:A21"/>
-    <mergeCell ref="B10:B20"/>
+    <mergeCell ref="B9:B20"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="A22:A43"/>
     <mergeCell ref="B22:B32"/>
@@ -3681,7 +3709,7 @@
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
-      <c r="F10" s="54"/>
+      <c r="F10" s="56"/>
       <c r="G10" s="15"/>
     </row>
     <row r="11" ht="14.25">
@@ -3692,7 +3720,7 @@
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
-      <c r="F11" s="54"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="15"/>
     </row>
     <row r="12" ht="14.25">
@@ -3703,7 +3731,7 @@
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
-      <c r="F12" s="54"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="15"/>
     </row>
     <row r="13" ht="14.25">
@@ -3714,7 +3742,7 @@
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
-      <c r="F13" s="54"/>
+      <c r="F13" s="56"/>
       <c r="G13" s="15"/>
     </row>
     <row r="14" ht="14.25">
@@ -3725,7 +3753,7 @@
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
-      <c r="F14" s="54"/>
+      <c r="F14" s="56"/>
       <c r="G14" s="15"/>
     </row>
     <row r="15" ht="14.25">
@@ -3736,7 +3764,7 @@
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
-      <c r="F15" s="54"/>
+      <c r="F15" s="56"/>
       <c r="G15" s="15"/>
     </row>
     <row r="16" ht="14.25">
@@ -3747,7 +3775,7 @@
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
-      <c r="F16" s="54"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="15"/>
     </row>
     <row r="17" ht="14.25">
@@ -3758,7 +3786,7 @@
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
-      <c r="F17" s="54"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="15"/>
     </row>
     <row r="18" ht="14.25">
@@ -3804,7 +3832,7 @@
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
-      <c r="F21" s="49"/>
+      <c r="F21" s="50"/>
       <c r="G21" s="34"/>
     </row>
     <row r="22" ht="14.25">
@@ -3815,7 +3843,7 @@
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
-      <c r="F22" s="49"/>
+      <c r="F22" s="50"/>
       <c r="G22" s="15"/>
     </row>
     <row r="23" ht="14.25">
@@ -3826,7 +3854,7 @@
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="35"/>
-      <c r="F23" s="49"/>
+      <c r="F23" s="50"/>
       <c r="G23" s="15"/>
     </row>
     <row r="24" ht="14.25">
@@ -3837,7 +3865,7 @@
       </c>
       <c r="D24" s="35"/>
       <c r="E24" s="35"/>
-      <c r="F24" s="49"/>
+      <c r="F24" s="50"/>
       <c r="G24" s="15"/>
     </row>
     <row r="25" ht="14.25">
@@ -3848,7 +3876,7 @@
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="36"/>
-      <c r="F25" s="50"/>
+      <c r="F25" s="51"/>
       <c r="G25" s="15"/>
     </row>
     <row r="26" ht="14.25">
@@ -3859,7 +3887,7 @@
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="38"/>
-      <c r="F26" s="51"/>
+      <c r="F26" s="52"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" ht="14.25">
@@ -3914,7 +3942,7 @@
       </c>
       <c r="D31" s="42"/>
       <c r="E31" s="42"/>
-      <c r="F31" s="52"/>
+      <c r="F31" s="54"/>
       <c r="G31" s="15"/>
     </row>
     <row r="32" ht="14.25">
@@ -3925,7 +3953,7 @@
       <c r="C32" s="44"/>
       <c r="D32" s="44"/>
       <c r="E32" s="44"/>
-      <c r="F32" s="53"/>
+      <c r="F32" s="55"/>
       <c r="G32" s="15"/>
     </row>
     <row r="33" ht="14.25">
@@ -3951,7 +3979,7 @@
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="26"/>
-      <c r="F34" s="54"/>
+      <c r="F34" s="56"/>
       <c r="G34" s="15"/>
     </row>
     <row r="35" ht="14.25">
@@ -3962,7 +3990,7 @@
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="26"/>
-      <c r="F35" s="54"/>
+      <c r="F35" s="56"/>
       <c r="G35" s="15"/>
     </row>
     <row r="36" ht="14.25">
@@ -3973,7 +4001,7 @@
       </c>
       <c r="D36" s="26"/>
       <c r="E36" s="26"/>
-      <c r="F36" s="54"/>
+      <c r="F36" s="56"/>
       <c r="G36" s="15"/>
     </row>
     <row r="37" ht="14.25">
@@ -3995,7 +4023,7 @@
       </c>
       <c r="D38" s="35"/>
       <c r="E38" s="35"/>
-      <c r="F38" s="54"/>
+      <c r="F38" s="56"/>
       <c r="G38" s="15"/>
     </row>
     <row r="39" ht="14.25">
@@ -4006,7 +4034,7 @@
       </c>
       <c r="D39" s="35"/>
       <c r="E39" s="35"/>
-      <c r="F39" s="54"/>
+      <c r="F39" s="56"/>
       <c r="G39" s="15"/>
     </row>
     <row r="40" ht="14.25">
@@ -4017,7 +4045,7 @@
       </c>
       <c r="D40" s="35"/>
       <c r="E40" s="35"/>
-      <c r="F40" s="54"/>
+      <c r="F40" s="56"/>
       <c r="G40" s="15"/>
     </row>
     <row r="41" ht="14.25">
@@ -4028,7 +4056,7 @@
       </c>
       <c r="D41" s="35"/>
       <c r="E41" s="35"/>
-      <c r="F41" s="54"/>
+      <c r="F41" s="56"/>
       <c r="G41" s="15"/>
     </row>
     <row r="42" ht="14.25">
@@ -4039,7 +4067,7 @@
       </c>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
-      <c r="F42" s="54"/>
+      <c r="F42" s="56"/>
       <c r="G42" s="15"/>
     </row>
     <row r="43" ht="14.25">
@@ -4063,7 +4091,7 @@
       </c>
       <c r="D44" s="35"/>
       <c r="E44" s="35"/>
-      <c r="F44" s="49"/>
+      <c r="F44" s="50"/>
       <c r="G44" s="34"/>
     </row>
     <row r="45" ht="14.25">
@@ -4074,7 +4102,7 @@
       </c>
       <c r="D45" s="35"/>
       <c r="E45" s="35"/>
-      <c r="F45" s="49"/>
+      <c r="F45" s="50"/>
       <c r="G45" s="15"/>
     </row>
     <row r="46" ht="14.25">
@@ -4151,7 +4179,7 @@
       </c>
       <c r="D52" s="35"/>
       <c r="E52" s="35"/>
-      <c r="F52" s="49"/>
+      <c r="F52" s="50"/>
       <c r="G52" s="15"/>
     </row>
     <row r="53" ht="14.25">
@@ -4173,7 +4201,7 @@
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="26"/>
-      <c r="F54" s="54">
+      <c r="F54" s="56">
         <f>SUM(F44:F53)</f>
         <v>0</v>
       </c>
@@ -4187,7 +4215,7 @@
       <c r="C55" s="44"/>
       <c r="D55" s="44"/>
       <c r="E55" s="44"/>
-      <c r="F55" s="53"/>
+      <c r="F55" s="55"/>
       <c r="G55" s="15"/>
     </row>
   </sheetData>
@@ -4336,7 +4364,7 @@
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
-      <c r="F7" s="54"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="15"/>
     </row>
     <row r="8" ht="14.25">
@@ -4347,7 +4375,7 @@
       </c>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
-      <c r="F8" s="54"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="15"/>
     </row>
     <row r="9" ht="14.25">
@@ -4358,7 +4386,7 @@
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
-      <c r="F9" s="54"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="15"/>
     </row>
     <row r="10" ht="14.25">
@@ -4369,7 +4397,7 @@
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
-      <c r="F10" s="54"/>
+      <c r="F10" s="56"/>
       <c r="G10" s="15"/>
     </row>
     <row r="11" ht="14.25">
@@ -4380,7 +4408,7 @@
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
-      <c r="F11" s="54"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="15"/>
     </row>
     <row r="12" ht="14.25">
@@ -4391,7 +4419,7 @@
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
-      <c r="F12" s="54"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="15"/>
     </row>
     <row r="13" ht="14.25">
@@ -4402,7 +4430,7 @@
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
-      <c r="F13" s="54"/>
+      <c r="F13" s="56"/>
       <c r="G13" s="15"/>
     </row>
     <row r="14" ht="14.25">
@@ -4413,7 +4441,7 @@
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
-      <c r="F14" s="54"/>
+      <c r="F14" s="56"/>
       <c r="G14" s="15"/>
     </row>
     <row r="15" ht="14.25">
@@ -4459,7 +4487,7 @@
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="35"/>
-      <c r="F18" s="49"/>
+      <c r="F18" s="50"/>
       <c r="G18" s="34"/>
     </row>
     <row r="19" ht="14.25">
@@ -4470,7 +4498,7 @@
       </c>
       <c r="D19" s="35"/>
       <c r="E19" s="35"/>
-      <c r="F19" s="49"/>
+      <c r="F19" s="50"/>
       <c r="G19" s="15"/>
     </row>
     <row r="20" ht="14.25">
@@ -4481,7 +4509,7 @@
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="35"/>
-      <c r="F20" s="49"/>
+      <c r="F20" s="50"/>
       <c r="G20" s="15"/>
     </row>
     <row r="21" ht="14.25">
@@ -4492,7 +4520,7 @@
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
-      <c r="F21" s="49"/>
+      <c r="F21" s="50"/>
       <c r="G21" s="15"/>
     </row>
     <row r="22" ht="14.25">
@@ -4503,7 +4531,7 @@
       </c>
       <c r="D22" s="32"/>
       <c r="E22" s="36"/>
-      <c r="F22" s="50"/>
+      <c r="F22" s="51"/>
       <c r="G22" s="15"/>
     </row>
     <row r="23" ht="14.25">
@@ -4514,7 +4542,7 @@
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="38"/>
-      <c r="F23" s="51"/>
+      <c r="F23" s="52"/>
       <c r="G23" s="15"/>
     </row>
     <row r="24" ht="14.25">
@@ -4569,7 +4597,7 @@
       </c>
       <c r="D28" s="42"/>
       <c r="E28" s="42"/>
-      <c r="F28" s="52"/>
+      <c r="F28" s="54"/>
       <c r="G28" s="15"/>
     </row>
     <row r="29" ht="14.25">
@@ -4580,7 +4608,7 @@
       <c r="C29" s="44"/>
       <c r="D29" s="44"/>
       <c r="E29" s="44"/>
-      <c r="F29" s="53"/>
+      <c r="F29" s="55"/>
       <c r="G29" s="15"/>
     </row>
     <row r="30" ht="14.25">
@@ -4606,7 +4634,7 @@
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="26"/>
-      <c r="F31" s="54"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="15"/>
     </row>
     <row r="32" ht="14.25">
@@ -4617,7 +4645,7 @@
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="26"/>
-      <c r="F32" s="54"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="15"/>
     </row>
     <row r="33" ht="14.25">
@@ -4628,7 +4656,7 @@
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="26"/>
-      <c r="F33" s="54"/>
+      <c r="F33" s="56"/>
       <c r="G33" s="15"/>
     </row>
     <row r="34" ht="14.25">
@@ -4650,7 +4678,7 @@
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="35"/>
-      <c r="F35" s="54"/>
+      <c r="F35" s="56"/>
       <c r="G35" s="15"/>
     </row>
     <row r="36" ht="14.25">
@@ -4661,7 +4689,7 @@
       </c>
       <c r="D36" s="35"/>
       <c r="E36" s="35"/>
-      <c r="F36" s="54"/>
+      <c r="F36" s="56"/>
       <c r="G36" s="15"/>
     </row>
     <row r="37" ht="14.25">
@@ -4672,7 +4700,7 @@
       </c>
       <c r="D37" s="35"/>
       <c r="E37" s="35"/>
-      <c r="F37" s="54"/>
+      <c r="F37" s="56"/>
       <c r="G37" s="15"/>
     </row>
     <row r="38" ht="14.25">
@@ -4683,7 +4711,7 @@
       </c>
       <c r="D38" s="35"/>
       <c r="E38" s="35"/>
-      <c r="F38" s="54"/>
+      <c r="F38" s="56"/>
       <c r="G38" s="15"/>
     </row>
     <row r="39" ht="14.25">
@@ -4694,7 +4722,7 @@
       </c>
       <c r="D39" s="26"/>
       <c r="E39" s="26"/>
-      <c r="F39" s="54"/>
+      <c r="F39" s="56"/>
       <c r="G39" s="15"/>
     </row>
     <row r="40" ht="14.25">
@@ -4718,7 +4746,7 @@
       </c>
       <c r="D41" s="35"/>
       <c r="E41" s="35"/>
-      <c r="F41" s="49"/>
+      <c r="F41" s="50"/>
       <c r="G41" s="34"/>
     </row>
     <row r="42" ht="14.25">
@@ -4729,7 +4757,7 @@
       </c>
       <c r="D42" s="35"/>
       <c r="E42" s="35"/>
-      <c r="F42" s="49"/>
+      <c r="F42" s="50"/>
       <c r="G42" s="15"/>
     </row>
     <row r="43" ht="14.25">
@@ -4806,7 +4834,7 @@
       </c>
       <c r="D49" s="35"/>
       <c r="E49" s="35"/>
-      <c r="F49" s="49"/>
+      <c r="F49" s="50"/>
       <c r="G49" s="15"/>
     </row>
     <row r="50" ht="14.25">
@@ -4828,7 +4856,7 @@
       </c>
       <c r="D51" s="26"/>
       <c r="E51" s="26"/>
-      <c r="F51" s="54">
+      <c r="F51" s="56">
         <f>SUM(F41:F50)</f>
         <v>0</v>
       </c>
@@ -4842,7 +4870,7 @@
       <c r="C52" s="44"/>
       <c r="D52" s="44"/>
       <c r="E52" s="44"/>
-      <c r="F52" s="53"/>
+      <c r="F52" s="55"/>
       <c r="G52" s="15"/>
     </row>
   </sheetData>
@@ -5049,7 +5077,7 @@
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
-      <c r="F10" s="54"/>
+      <c r="F10" s="56"/>
       <c r="G10" s="15"/>
     </row>
     <row r="11" s="0" customFormat="1" ht="14.25">
@@ -5060,7 +5088,7 @@
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
-      <c r="F11" s="54"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="15"/>
     </row>
     <row r="12" s="0" customFormat="1" ht="14.25">
@@ -5071,7 +5099,7 @@
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
-      <c r="F12" s="54"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="15"/>
     </row>
     <row r="13" s="0" customFormat="1" ht="14.25">
@@ -5082,7 +5110,7 @@
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
-      <c r="F13" s="54"/>
+      <c r="F13" s="56"/>
       <c r="G13" s="15"/>
     </row>
     <row r="14" s="0" customFormat="1" ht="14.25">
@@ -5093,7 +5121,7 @@
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
-      <c r="F14" s="54"/>
+      <c r="F14" s="56"/>
       <c r="G14" s="15"/>
     </row>
     <row r="15" s="0" customFormat="1" ht="14.25">
@@ -5104,7 +5132,7 @@
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
-      <c r="F15" s="54"/>
+      <c r="F15" s="56"/>
       <c r="G15" s="15"/>
     </row>
     <row r="16" s="0" customFormat="1" ht="14.25">
@@ -5115,7 +5143,7 @@
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
-      <c r="F16" s="54"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="15"/>
     </row>
     <row r="17" s="0" customFormat="1" ht="14.25">
@@ -5126,7 +5154,7 @@
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
-      <c r="F17" s="54"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="15"/>
     </row>
     <row r="18" s="0" customFormat="1" ht="14.25">
@@ -5172,7 +5200,7 @@
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
-      <c r="F21" s="49"/>
+      <c r="F21" s="50"/>
       <c r="G21" s="34"/>
     </row>
     <row r="22" s="0" customFormat="1" ht="14.25">
@@ -5183,7 +5211,7 @@
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
-      <c r="F22" s="49"/>
+      <c r="F22" s="50"/>
       <c r="G22" s="15"/>
     </row>
     <row r="23" s="0" customFormat="1" ht="14.25">
@@ -5194,7 +5222,7 @@
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="35"/>
-      <c r="F23" s="49"/>
+      <c r="F23" s="50"/>
       <c r="G23" s="15"/>
     </row>
     <row r="24" s="0" customFormat="1" ht="14.25">
@@ -5205,7 +5233,7 @@
       </c>
       <c r="D24" s="35"/>
       <c r="E24" s="35"/>
-      <c r="F24" s="49"/>
+      <c r="F24" s="50"/>
       <c r="G24" s="15"/>
     </row>
     <row r="25" s="0" customFormat="1" ht="14.25">
@@ -5216,7 +5244,7 @@
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="36"/>
-      <c r="F25" s="50"/>
+      <c r="F25" s="51"/>
       <c r="G25" s="15"/>
     </row>
     <row r="26" s="0" customFormat="1" ht="14.25">
@@ -5227,7 +5255,7 @@
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="38"/>
-      <c r="F26" s="51"/>
+      <c r="F26" s="52"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" s="0" customFormat="1" ht="14.25">
@@ -5282,7 +5310,7 @@
       </c>
       <c r="D31" s="42"/>
       <c r="E31" s="42"/>
-      <c r="F31" s="52"/>
+      <c r="F31" s="54"/>
       <c r="G31" s="15"/>
     </row>
     <row r="32" s="0" customFormat="1" ht="14.25">
@@ -5293,7 +5321,7 @@
       <c r="C32" s="44"/>
       <c r="D32" s="44"/>
       <c r="E32" s="44"/>
-      <c r="F32" s="53"/>
+      <c r="F32" s="55"/>
       <c r="G32" s="15"/>
     </row>
     <row r="33" s="0" customFormat="1" ht="14.25">
@@ -5319,7 +5347,7 @@
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="26"/>
-      <c r="F34" s="54"/>
+      <c r="F34" s="56"/>
       <c r="G34" s="15"/>
     </row>
     <row r="35" s="0" customFormat="1" ht="14.25">
@@ -5330,7 +5358,7 @@
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="26"/>
-      <c r="F35" s="54"/>
+      <c r="F35" s="56"/>
       <c r="G35" s="15"/>
     </row>
     <row r="36" s="0" customFormat="1" ht="14.25">
@@ -5341,7 +5369,7 @@
       </c>
       <c r="D36" s="26"/>
       <c r="E36" s="26"/>
-      <c r="F36" s="54"/>
+      <c r="F36" s="56"/>
       <c r="G36" s="15"/>
     </row>
     <row r="37" s="0" customFormat="1" ht="14.25">
@@ -5363,7 +5391,7 @@
       </c>
       <c r="D38" s="35"/>
       <c r="E38" s="35"/>
-      <c r="F38" s="54"/>
+      <c r="F38" s="56"/>
       <c r="G38" s="15"/>
     </row>
     <row r="39" s="0" customFormat="1" ht="14.25">
@@ -5374,7 +5402,7 @@
       </c>
       <c r="D39" s="35"/>
       <c r="E39" s="35"/>
-      <c r="F39" s="54"/>
+      <c r="F39" s="56"/>
       <c r="G39" s="15"/>
     </row>
     <row r="40" s="0" customFormat="1" ht="14.25">
@@ -5385,7 +5413,7 @@
       </c>
       <c r="D40" s="35"/>
       <c r="E40" s="35"/>
-      <c r="F40" s="54"/>
+      <c r="F40" s="56"/>
       <c r="G40" s="15"/>
     </row>
     <row r="41" s="0" customFormat="1" ht="14.25">
@@ -5396,7 +5424,7 @@
       </c>
       <c r="D41" s="35"/>
       <c r="E41" s="35"/>
-      <c r="F41" s="54"/>
+      <c r="F41" s="56"/>
       <c r="G41" s="15"/>
     </row>
     <row r="42" s="0" customFormat="1" ht="14.25">
@@ -5407,7 +5435,7 @@
       </c>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
-      <c r="F42" s="54"/>
+      <c r="F42" s="56"/>
       <c r="G42" s="15"/>
     </row>
     <row r="43" s="0" customFormat="1" ht="14.25">
@@ -5431,7 +5459,7 @@
       </c>
       <c r="D44" s="35"/>
       <c r="E44" s="35"/>
-      <c r="F44" s="49"/>
+      <c r="F44" s="50"/>
       <c r="G44" s="34"/>
     </row>
     <row r="45" s="0" customFormat="1" ht="14.25">
@@ -5442,7 +5470,7 @@
       </c>
       <c r="D45" s="35"/>
       <c r="E45" s="35"/>
-      <c r="F45" s="49"/>
+      <c r="F45" s="50"/>
       <c r="G45" s="15"/>
     </row>
     <row r="46" s="0" customFormat="1" ht="14.25">
@@ -5519,7 +5547,7 @@
       </c>
       <c r="D52" s="35"/>
       <c r="E52" s="35"/>
-      <c r="F52" s="49"/>
+      <c r="F52" s="50"/>
       <c r="G52" s="15"/>
     </row>
     <row r="53" s="0" customFormat="1" ht="14.25">
@@ -5541,7 +5569,7 @@
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="26"/>
-      <c r="F54" s="54"/>
+      <c r="F54" s="56"/>
       <c r="G54" s="15"/>
     </row>
     <row r="55" s="0" customFormat="1" ht="14.25">
@@ -5552,7 +5580,7 @@
       <c r="C55" s="44"/>
       <c r="D55" s="44"/>
       <c r="E55" s="44"/>
-      <c r="F55" s="53"/>
+      <c r="F55" s="55"/>
       <c r="G55" s="15"/>
     </row>
     <row r="56" s="0" customFormat="1"/>
@@ -5709,7 +5737,7 @@
     <row r="5" ht="28.5">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="57" t="s">
         <v>48</v>
       </c>
       <c r="D5" s="15">
@@ -5797,7 +5825,7 @@
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
-      <c r="F10" s="54"/>
+      <c r="F10" s="56"/>
       <c r="G10" s="15"/>
     </row>
     <row r="11" ht="14.25">
@@ -5808,7 +5836,7 @@
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
-      <c r="F11" s="54"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="15"/>
     </row>
     <row r="12" ht="14.25">
@@ -5819,7 +5847,7 @@
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
-      <c r="F12" s="54"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="15"/>
     </row>
     <row r="13" ht="14.25">
@@ -5830,7 +5858,7 @@
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
-      <c r="F13" s="54"/>
+      <c r="F13" s="56"/>
       <c r="G13" s="15"/>
     </row>
     <row r="14" ht="14.25">
@@ -5841,7 +5869,7 @@
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
-      <c r="F14" s="54"/>
+      <c r="F14" s="56"/>
       <c r="G14" s="15"/>
     </row>
     <row r="15" ht="14.25">
@@ -5852,7 +5880,7 @@
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
-      <c r="F15" s="54"/>
+      <c r="F15" s="56"/>
       <c r="G15" s="15"/>
     </row>
     <row r="16" ht="14.25">
@@ -5863,7 +5891,7 @@
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
-      <c r="F16" s="54"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="15"/>
     </row>
     <row r="17" ht="14.25">
@@ -5874,7 +5902,7 @@
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
-      <c r="F17" s="54"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="15"/>
     </row>
     <row r="18" ht="14.25">
@@ -5920,7 +5948,7 @@
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
-      <c r="F21" s="49"/>
+      <c r="F21" s="50"/>
       <c r="G21" s="34"/>
     </row>
     <row r="22" ht="14.25">
@@ -5931,7 +5959,7 @@
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
-      <c r="F22" s="49"/>
+      <c r="F22" s="50"/>
       <c r="G22" s="15"/>
     </row>
     <row r="23" ht="14.25">
@@ -5942,7 +5970,7 @@
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="35"/>
-      <c r="F23" s="49"/>
+      <c r="F23" s="50"/>
       <c r="G23" s="15"/>
     </row>
     <row r="24" ht="14.25">
@@ -5953,7 +5981,7 @@
       </c>
       <c r="D24" s="35"/>
       <c r="E24" s="35"/>
-      <c r="F24" s="49"/>
+      <c r="F24" s="50"/>
       <c r="G24" s="15"/>
     </row>
     <row r="25" ht="14.25">
@@ -5964,7 +5992,7 @@
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="36"/>
-      <c r="F25" s="50"/>
+      <c r="F25" s="51"/>
       <c r="G25" s="15"/>
     </row>
     <row r="26" ht="14.25">
@@ -5975,7 +6003,7 @@
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="38"/>
-      <c r="F26" s="51"/>
+      <c r="F26" s="52"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" ht="14.25">
@@ -6030,7 +6058,7 @@
       </c>
       <c r="D31" s="42"/>
       <c r="E31" s="42"/>
-      <c r="F31" s="52"/>
+      <c r="F31" s="54"/>
       <c r="G31" s="15"/>
     </row>
     <row r="32" ht="14.25">
@@ -6041,7 +6069,7 @@
       <c r="C32" s="44"/>
       <c r="D32" s="44"/>
       <c r="E32" s="44"/>
-      <c r="F32" s="53"/>
+      <c r="F32" s="55"/>
       <c r="G32" s="15"/>
     </row>
     <row r="33" ht="14.25">
@@ -6092,7 +6120,7 @@
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="26"/>
-      <c r="F35" s="54"/>
+      <c r="F35" s="56"/>
       <c r="G35" s="15"/>
     </row>
     <row r="36" ht="14.25">
@@ -6103,7 +6131,7 @@
       </c>
       <c r="D36" s="26"/>
       <c r="E36" s="26"/>
-      <c r="F36" s="54"/>
+      <c r="F36" s="56"/>
       <c r="G36" s="15"/>
     </row>
     <row r="37" ht="14.25">
@@ -6114,7 +6142,7 @@
       </c>
       <c r="D37" s="26"/>
       <c r="E37" s="26"/>
-      <c r="F37" s="54"/>
+      <c r="F37" s="56"/>
       <c r="G37" s="15"/>
     </row>
     <row r="38" ht="14.25">
@@ -6136,7 +6164,7 @@
       </c>
       <c r="D39" s="35"/>
       <c r="E39" s="35"/>
-      <c r="F39" s="54"/>
+      <c r="F39" s="56"/>
       <c r="G39" s="15"/>
     </row>
     <row r="40" ht="14.25">
@@ -6147,7 +6175,7 @@
       </c>
       <c r="D40" s="35"/>
       <c r="E40" s="35"/>
-      <c r="F40" s="54"/>
+      <c r="F40" s="56"/>
       <c r="G40" s="15"/>
     </row>
     <row r="41" ht="14.25">
@@ -6158,7 +6186,7 @@
       </c>
       <c r="D41" s="35"/>
       <c r="E41" s="35"/>
-      <c r="F41" s="54"/>
+      <c r="F41" s="56"/>
       <c r="G41" s="15"/>
     </row>
     <row r="42" ht="14.25">
@@ -6169,7 +6197,7 @@
       </c>
       <c r="D42" s="35"/>
       <c r="E42" s="35"/>
-      <c r="F42" s="54"/>
+      <c r="F42" s="56"/>
       <c r="G42" s="15"/>
     </row>
     <row r="43" ht="14.25">
@@ -6180,7 +6208,7 @@
       </c>
       <c r="D43" s="26"/>
       <c r="E43" s="26"/>
-      <c r="F43" s="54"/>
+      <c r="F43" s="56"/>
       <c r="G43" s="15"/>
     </row>
     <row r="44" ht="14.25">
@@ -6207,7 +6235,7 @@
       </c>
       <c r="D45" s="35"/>
       <c r="E45" s="35"/>
-      <c r="F45" s="49"/>
+      <c r="F45" s="50"/>
       <c r="G45" s="34"/>
     </row>
     <row r="46" ht="14.25">
@@ -6218,7 +6246,7 @@
       </c>
       <c r="D46" s="35"/>
       <c r="E46" s="35"/>
-      <c r="F46" s="49"/>
+      <c r="F46" s="50"/>
       <c r="G46" s="15"/>
     </row>
     <row r="47" ht="14.25">
@@ -6295,7 +6323,7 @@
       </c>
       <c r="D53" s="35"/>
       <c r="E53" s="35"/>
-      <c r="F53" s="49"/>
+      <c r="F53" s="50"/>
       <c r="G53" s="15"/>
     </row>
     <row r="54" ht="14.25">
@@ -6317,7 +6345,7 @@
       </c>
       <c r="D55" s="26"/>
       <c r="E55" s="26"/>
-      <c r="F55" s="54"/>
+      <c r="F55" s="56"/>
       <c r="G55" s="15"/>
     </row>
     <row r="56" ht="14.25">
@@ -6328,7 +6356,7 @@
       <c r="C56" s="44"/>
       <c r="D56" s="44"/>
       <c r="E56" s="44"/>
-      <c r="F56" s="53"/>
+      <c r="F56" s="55"/>
       <c r="G56" s="15"/>
     </row>
   </sheetData>
@@ -6496,7 +6524,7 @@
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
-      <c r="F10" s="54"/>
+      <c r="F10" s="56"/>
       <c r="G10" s="15"/>
     </row>
     <row r="11" ht="14.25">
@@ -6507,7 +6535,7 @@
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
-      <c r="F11" s="54"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="15"/>
     </row>
     <row r="12" ht="14.25">
@@ -6518,7 +6546,7 @@
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
-      <c r="F12" s="54"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="15"/>
     </row>
     <row r="13" ht="14.25">
@@ -6529,7 +6557,7 @@
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
-      <c r="F13" s="54"/>
+      <c r="F13" s="56"/>
       <c r="G13" s="15"/>
     </row>
     <row r="14" ht="14.25">
@@ -6540,7 +6568,7 @@
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
-      <c r="F14" s="54"/>
+      <c r="F14" s="56"/>
       <c r="G14" s="15"/>
     </row>
     <row r="15" ht="14.25">
@@ -6551,7 +6579,7 @@
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
-      <c r="F15" s="54"/>
+      <c r="F15" s="56"/>
       <c r="G15" s="15"/>
     </row>
     <row r="16" ht="14.25">
@@ -6562,7 +6590,7 @@
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
-      <c r="F16" s="54"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="15"/>
     </row>
     <row r="17" ht="14.25">
@@ -6573,7 +6601,7 @@
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
-      <c r="F17" s="54"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="15"/>
     </row>
     <row r="18" ht="14.25">
@@ -6619,7 +6647,7 @@
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
-      <c r="F21" s="49"/>
+      <c r="F21" s="50"/>
       <c r="G21" s="34"/>
     </row>
     <row r="22" ht="14.25">
@@ -6630,7 +6658,7 @@
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
-      <c r="F22" s="49"/>
+      <c r="F22" s="50"/>
       <c r="G22" s="15"/>
     </row>
     <row r="23" ht="14.25">
@@ -6641,7 +6669,7 @@
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="35"/>
-      <c r="F23" s="49"/>
+      <c r="F23" s="50"/>
       <c r="G23" s="15"/>
     </row>
     <row r="24" ht="14.25">
@@ -6652,7 +6680,7 @@
       </c>
       <c r="D24" s="35"/>
       <c r="E24" s="35"/>
-      <c r="F24" s="49"/>
+      <c r="F24" s="50"/>
       <c r="G24" s="15"/>
     </row>
     <row r="25" ht="14.25">
@@ -6663,7 +6691,7 @@
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="36"/>
-      <c r="F25" s="50"/>
+      <c r="F25" s="51"/>
       <c r="G25" s="15"/>
     </row>
     <row r="26" ht="14.25">
@@ -6674,7 +6702,7 @@
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="38"/>
-      <c r="F26" s="51"/>
+      <c r="F26" s="52"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" ht="14.25">
@@ -6729,7 +6757,7 @@
       </c>
       <c r="D31" s="42"/>
       <c r="E31" s="42"/>
-      <c r="F31" s="52"/>
+      <c r="F31" s="54"/>
       <c r="G31" s="15"/>
     </row>
     <row r="32" ht="14.25">
@@ -6740,7 +6768,7 @@
       <c r="C32" s="44"/>
       <c r="D32" s="44"/>
       <c r="E32" s="44"/>
-      <c r="F32" s="53"/>
+      <c r="F32" s="55"/>
       <c r="G32" s="15"/>
     </row>
     <row r="33" ht="14.25">
@@ -6766,7 +6794,7 @@
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="26"/>
-      <c r="F34" s="54"/>
+      <c r="F34" s="56"/>
       <c r="G34" s="15"/>
     </row>
     <row r="35" ht="14.25">
@@ -6777,7 +6805,7 @@
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="26"/>
-      <c r="F35" s="54"/>
+      <c r="F35" s="56"/>
       <c r="G35" s="15"/>
     </row>
     <row r="36" ht="14.25">
@@ -6788,7 +6816,7 @@
       </c>
       <c r="D36" s="26"/>
       <c r="E36" s="26"/>
-      <c r="F36" s="54"/>
+      <c r="F36" s="56"/>
       <c r="G36" s="15"/>
     </row>
     <row r="37" ht="14.25">
@@ -6810,7 +6838,7 @@
       </c>
       <c r="D38" s="35"/>
       <c r="E38" s="35"/>
-      <c r="F38" s="54"/>
+      <c r="F38" s="56"/>
       <c r="G38" s="15"/>
     </row>
     <row r="39" ht="14.25">
@@ -6821,7 +6849,7 @@
       </c>
       <c r="D39" s="35"/>
       <c r="E39" s="35"/>
-      <c r="F39" s="54"/>
+      <c r="F39" s="56"/>
       <c r="G39" s="15"/>
     </row>
     <row r="40" ht="14.25">
@@ -6832,7 +6860,7 @@
       </c>
       <c r="D40" s="35"/>
       <c r="E40" s="35"/>
-      <c r="F40" s="54"/>
+      <c r="F40" s="56"/>
       <c r="G40" s="15"/>
     </row>
     <row r="41" ht="14.25">
@@ -6843,7 +6871,7 @@
       </c>
       <c r="D41" s="35"/>
       <c r="E41" s="35"/>
-      <c r="F41" s="54"/>
+      <c r="F41" s="56"/>
       <c r="G41" s="15"/>
     </row>
     <row r="42" ht="14.25">
@@ -6854,7 +6882,7 @@
       </c>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
-      <c r="F42" s="54"/>
+      <c r="F42" s="56"/>
       <c r="G42" s="15"/>
     </row>
     <row r="43" ht="14.25">
@@ -6878,7 +6906,7 @@
       </c>
       <c r="D44" s="35"/>
       <c r="E44" s="35"/>
-      <c r="F44" s="49"/>
+      <c r="F44" s="50"/>
       <c r="G44" s="34"/>
     </row>
     <row r="45" ht="14.25">
@@ -6889,7 +6917,7 @@
       </c>
       <c r="D45" s="35"/>
       <c r="E45" s="35"/>
-      <c r="F45" s="49"/>
+      <c r="F45" s="50"/>
       <c r="G45" s="15"/>
     </row>
     <row r="46" ht="14.25">
@@ -6966,7 +6994,7 @@
       </c>
       <c r="D52" s="35"/>
       <c r="E52" s="35"/>
-      <c r="F52" s="49"/>
+      <c r="F52" s="50"/>
       <c r="G52" s="15"/>
     </row>
     <row r="53" ht="14.25">
@@ -6988,7 +7016,7 @@
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="26"/>
-      <c r="F54" s="54"/>
+      <c r="F54" s="56"/>
       <c r="G54" s="15"/>
     </row>
     <row r="55" s="0" customFormat="1" ht="14.25">
@@ -6999,7 +7027,7 @@
       <c r="C55" s="44"/>
       <c r="D55" s="44"/>
       <c r="E55" s="44"/>
-      <c r="F55" s="53"/>
+      <c r="F55" s="55"/>
       <c r="G55" s="15"/>
     </row>
     <row r="56" s="0" customFormat="1"/>
@@ -7039,17 +7067,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="56" width="8.875"/>
-    <col customWidth="1" min="2" max="2" style="56" width="22.140625"/>
-    <col customWidth="1" min="3" max="3" style="56" width="20.274999999999999"/>
-    <col customWidth="1" min="4" max="4" style="56" width="19.125"/>
-    <col customWidth="1" min="5" max="5" style="56" width="26.875"/>
-    <col customWidth="1" min="6" max="6" style="56" width="22.758333333333301"/>
-    <col customWidth="1" min="7" max="7" style="56" width="20.758333333333301"/>
-    <col customWidth="1" min="8" max="8" style="56" width="18.375"/>
-    <col min="9" max="10" style="56" width="9"/>
-    <col customWidth="1" min="11" max="11" style="56" width="12.758333333333301"/>
-    <col min="12" max="16384" style="56" width="9"/>
+    <col customWidth="1" min="1" max="1" style="58" width="8.875"/>
+    <col customWidth="1" min="2" max="2" style="58" width="22.140625"/>
+    <col customWidth="1" min="3" max="3" style="58" width="20.274999999999999"/>
+    <col customWidth="1" min="4" max="4" style="58" width="19.125"/>
+    <col customWidth="1" min="5" max="5" style="58" width="26.875"/>
+    <col customWidth="1" min="6" max="6" style="58" width="22.758333333333301"/>
+    <col customWidth="1" min="7" max="7" style="58" width="20.758333333333301"/>
+    <col customWidth="1" min="8" max="8" style="58" width="18.375"/>
+    <col min="9" max="10" style="58" width="9"/>
+    <col customWidth="1" min="11" max="11" style="58" width="12.758333333333301"/>
+    <col min="12" max="16384" style="58" width="9"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25">
@@ -7062,7 +7090,7 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="13"/>
-      <c r="H1" s="57"/>
+      <c r="H1" s="59"/>
     </row>
     <row r="2" s="0" customFormat="1" ht="15">
       <c r="A2" s="14" t="s">
@@ -7198,7 +7226,7 @@
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
-      <c r="F10" s="54"/>
+      <c r="F10" s="56"/>
       <c r="G10" s="15"/>
     </row>
     <row r="11" s="0" customFormat="1" ht="15">
@@ -7209,7 +7237,7 @@
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
-      <c r="F11" s="54"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="15"/>
     </row>
     <row r="12" s="0" customFormat="1" ht="15">
@@ -7220,7 +7248,7 @@
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
-      <c r="F12" s="54"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="15"/>
     </row>
     <row r="13" s="0" customFormat="1" ht="15">
@@ -7231,7 +7259,7 @@
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
-      <c r="F13" s="54"/>
+      <c r="F13" s="56"/>
       <c r="G13" s="15"/>
     </row>
     <row r="14" s="0" customFormat="1" ht="15">
@@ -7242,7 +7270,7 @@
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
-      <c r="F14" s="54"/>
+      <c r="F14" s="56"/>
       <c r="G14" s="15"/>
     </row>
     <row r="15" s="0" customFormat="1" ht="15">
@@ -7253,7 +7281,7 @@
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
-      <c r="F15" s="54"/>
+      <c r="F15" s="56"/>
       <c r="G15" s="15"/>
     </row>
     <row r="16" s="0" customFormat="1" ht="15">
@@ -7264,7 +7292,7 @@
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
-      <c r="F16" s="54"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="15"/>
     </row>
     <row r="17" s="0" customFormat="1" ht="15">
@@ -7275,7 +7303,7 @@
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
-      <c r="F17" s="54"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="15"/>
     </row>
     <row r="18" s="0" customFormat="1" ht="15">
@@ -7321,7 +7349,7 @@
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
-      <c r="F21" s="49"/>
+      <c r="F21" s="50"/>
       <c r="G21" s="34"/>
     </row>
     <row r="22" s="0" customFormat="1" ht="15">
@@ -7332,7 +7360,7 @@
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
-      <c r="F22" s="49"/>
+      <c r="F22" s="50"/>
       <c r="G22" s="15"/>
     </row>
     <row r="23" s="0" customFormat="1" ht="15">
@@ -7343,7 +7371,7 @@
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="35"/>
-      <c r="F23" s="49"/>
+      <c r="F23" s="50"/>
       <c r="G23" s="15"/>
     </row>
     <row r="24" s="0" customFormat="1" ht="15">
@@ -7354,7 +7382,7 @@
       </c>
       <c r="D24" s="35"/>
       <c r="E24" s="35"/>
-      <c r="F24" s="49"/>
+      <c r="F24" s="50"/>
       <c r="G24" s="15"/>
     </row>
     <row r="25" s="0" customFormat="1" ht="15">
@@ -7365,7 +7393,7 @@
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="36"/>
-      <c r="F25" s="50"/>
+      <c r="F25" s="51"/>
       <c r="G25" s="15"/>
     </row>
     <row r="26" s="0" customFormat="1" ht="15">
@@ -7376,7 +7404,7 @@
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="38"/>
-      <c r="F26" s="51"/>
+      <c r="F26" s="52"/>
       <c r="G26" s="15"/>
     </row>
     <row r="27" s="0" customFormat="1" ht="15">
@@ -7431,7 +7459,7 @@
       </c>
       <c r="D31" s="42"/>
       <c r="E31" s="42"/>
-      <c r="F31" s="52"/>
+      <c r="F31" s="54"/>
       <c r="G31" s="15"/>
     </row>
     <row r="32" s="0" customFormat="1" ht="15">
@@ -7442,7 +7470,7 @@
       <c r="C32" s="44"/>
       <c r="D32" s="44"/>
       <c r="E32" s="44"/>
-      <c r="F32" s="53"/>
+      <c r="F32" s="55"/>
       <c r="G32" s="15"/>
     </row>
     <row r="33" s="0" customFormat="1" ht="15">
@@ -7468,7 +7496,7 @@
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="26"/>
-      <c r="F34" s="54"/>
+      <c r="F34" s="56"/>
       <c r="G34" s="15"/>
     </row>
     <row r="35" s="0" customFormat="1" ht="15">
@@ -7479,7 +7507,7 @@
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="26"/>
-      <c r="F35" s="54"/>
+      <c r="F35" s="56"/>
       <c r="G35" s="15"/>
     </row>
     <row r="36" s="0" customFormat="1" ht="15">
@@ -7490,7 +7518,7 @@
       </c>
       <c r="D36" s="26"/>
       <c r="E36" s="26"/>
-      <c r="F36" s="54"/>
+      <c r="F36" s="56"/>
       <c r="G36" s="15"/>
     </row>
     <row r="37" s="0" customFormat="1" ht="15">
@@ -7512,7 +7540,7 @@
       </c>
       <c r="D38" s="35"/>
       <c r="E38" s="35"/>
-      <c r="F38" s="54"/>
+      <c r="F38" s="56"/>
       <c r="G38" s="15"/>
     </row>
     <row r="39" s="0" customFormat="1" ht="15">
@@ -7523,7 +7551,7 @@
       </c>
       <c r="D39" s="35"/>
       <c r="E39" s="35"/>
-      <c r="F39" s="54"/>
+      <c r="F39" s="56"/>
       <c r="G39" s="15"/>
     </row>
     <row r="40" s="0" customFormat="1" ht="15">
@@ -7534,7 +7562,7 @@
       </c>
       <c r="D40" s="35"/>
       <c r="E40" s="35"/>
-      <c r="F40" s="54"/>
+      <c r="F40" s="56"/>
       <c r="G40" s="15"/>
     </row>
     <row r="41" s="0" customFormat="1" ht="15">
@@ -7545,7 +7573,7 @@
       </c>
       <c r="D41" s="35"/>
       <c r="E41" s="35"/>
-      <c r="F41" s="54"/>
+      <c r="F41" s="56"/>
       <c r="G41" s="15"/>
     </row>
     <row r="42" s="0" customFormat="1" ht="15">
@@ -7556,7 +7584,7 @@
       </c>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
-      <c r="F42" s="54"/>
+      <c r="F42" s="56"/>
       <c r="G42" s="15"/>
     </row>
     <row r="43" s="0" customFormat="1" ht="15">
@@ -7580,7 +7608,7 @@
       </c>
       <c r="D44" s="35"/>
       <c r="E44" s="35"/>
-      <c r="F44" s="49"/>
+      <c r="F44" s="50"/>
       <c r="G44" s="34"/>
     </row>
     <row r="45" s="0" customFormat="1" ht="15">
@@ -7591,7 +7619,7 @@
       </c>
       <c r="D45" s="35"/>
       <c r="E45" s="35"/>
-      <c r="F45" s="49"/>
+      <c r="F45" s="50"/>
       <c r="G45" s="15"/>
     </row>
     <row r="46" s="0" customFormat="1" ht="15">
@@ -7668,7 +7696,7 @@
       </c>
       <c r="D52" s="35"/>
       <c r="E52" s="35"/>
-      <c r="F52" s="49"/>
+      <c r="F52" s="50"/>
       <c r="G52" s="15"/>
     </row>
     <row r="53" s="0" customFormat="1" ht="15">
@@ -7690,7 +7718,7 @@
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="26"/>
-      <c r="F54" s="54"/>
+      <c r="F54" s="56"/>
       <c r="G54" s="15"/>
     </row>
     <row r="55" s="0" customFormat="1" ht="15">
@@ -7701,7 +7729,7 @@
       <c r="C55" s="44"/>
       <c r="D55" s="44"/>
       <c r="E55" s="44"/>
-      <c r="F55" s="53"/>
+      <c r="F55" s="55"/>
       <c r="G55" s="15"/>
     </row>
     <row r="56" s="0" customFormat="1"/>
@@ -7764,42 +7792,42 @@
     <row r="113" s="0" customFormat="1"/>
     <row r="114" s="0" customFormat="1"/>
     <row r="115" ht="14.25">
-      <c r="A115" s="58"/>
-      <c r="B115" s="58"/>
-      <c r="C115" s="58"/>
-      <c r="D115" s="58"/>
-      <c r="E115" s="58"/>
-      <c r="F115" s="59" t="s">
+      <c r="A115" s="60"/>
+      <c r="B115" s="60"/>
+      <c r="C115" s="60"/>
+      <c r="D115" s="60"/>
+      <c r="E115" s="60"/>
+      <c r="F115" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="G115" s="59"/>
+      <c r="G115" s="61"/>
     </row>
     <row r="116" ht="14.25">
-      <c r="A116" s="58"/>
-      <c r="B116" s="58"/>
-      <c r="C116" s="58"/>
-      <c r="D116" s="57"/>
-      <c r="E116" s="58"/>
-      <c r="F116" s="58"/>
-      <c r="G116" s="58"/>
+      <c r="A116" s="60"/>
+      <c r="B116" s="60"/>
+      <c r="C116" s="60"/>
+      <c r="D116" s="59"/>
+      <c r="E116" s="60"/>
+      <c r="F116" s="60"/>
+      <c r="G116" s="60"/>
     </row>
     <row r="117">
-      <c r="A117" s="57"/>
-      <c r="B117" s="57"/>
-      <c r="C117" s="57"/>
-      <c r="D117" s="57"/>
-      <c r="E117" s="57"/>
-      <c r="F117" s="57"/>
-      <c r="G117" s="60"/>
+      <c r="A117" s="59"/>
+      <c r="B117" s="59"/>
+      <c r="C117" s="59"/>
+      <c r="D117" s="59"/>
+      <c r="E117" s="59"/>
+      <c r="F117" s="59"/>
+      <c r="G117" s="62"/>
     </row>
     <row r="119">
-      <c r="A119" s="57"/>
-      <c r="B119" s="57"/>
-      <c r="C119" s="57"/>
-      <c r="D119" s="61"/>
-      <c r="E119" s="57"/>
-      <c r="F119" s="57"/>
-      <c r="G119" s="57"/>
+      <c r="A119" s="59"/>
+      <c r="B119" s="59"/>
+      <c r="C119" s="59"/>
+      <c r="D119" s="63"/>
+      <c r="E119" s="59"/>
+      <c r="F119" s="59"/>
+      <c r="G119" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>